<commit_message>
RR-communication mappings and added GuidanceResponse and Parameters mapping as options
</commit_message>
<xml_diff>
--- a/docs/rr-communication.xlsx
+++ b/docs/rr-communication.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="405">
   <si>
     <t>Path</t>
   </si>
@@ -634,7 +634,7 @@
     <t>Communication.recipient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization}
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-organization}
 </t>
   </si>
   <si>
@@ -975,14 +975,17 @@
 </t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/StructureDefinition/Encounter}
-Reference {http://hl7.org/fhir/StructureDefinition/EpisodeOfCare}</t>
-  </si>
-  <si>
-    <t>Encounter or episode leading to message</t>
-  </si>
-  <si>
-    <t>The encounter within which the communication was sent.</t>
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/eicr-encounter}
+</t>
+  </si>
+  <si>
+    <t>eICR encompassing encounter ID</t>
+  </si>
+  <si>
+    <t>The encompassing encounter ID from the eICR that generatedthe Reportability Response.</t>
+  </si>
+  <si>
+    <t>eICR Encompassing Encounter ID</t>
   </si>
   <si>
     <t>Event.context</t>
@@ -1030,7 +1033,7 @@
   </si>
   <si>
     <t>Reference {http://hl7.org/fhir/StructureDefinition/Device}
-Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization}Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner}</t>
+Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-organization}Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner}</t>
   </si>
   <si>
     <t>Message sender</t>
@@ -8554,7 +8557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65" hidden="true">
+    <row r="65">
       <c r="A65" t="s" s="2">
         <v>303</v>
       </c>
@@ -8570,7 +8573,7 @@
         <v>51</v>
       </c>
       <c r="G65" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H65" t="s" s="2">
         <v>40</v>
@@ -8651,10 +8654,10 @@
         <v>40</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>40</v>
+        <v>308</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>254</v>
@@ -8665,7 +8668,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8688,13 +8691,13 @@
         <v>40</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8745,7 +8748,7 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -8763,10 +8766,10 @@
         <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>40</v>
@@ -8774,7 +8777,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8797,13 +8800,13 @@
         <v>40</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8854,7 +8857,7 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -8869,13 +8872,13 @@
         <v>40</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>40</v>
@@ -8883,11 +8886,11 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
@@ -8906,16 +8909,16 @@
         <v>40</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -8965,7 +8968,7 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
@@ -8980,13 +8983,13 @@
         <v>40</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>40</v>
@@ -8994,7 +8997,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9103,7 +9106,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9214,13 +9217,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C71" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -9239,7 +9242,7 @@
         <v>40</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K71" t="s" s="2">
         <v>96</v>
@@ -9248,7 +9251,7 @@
         <v>97</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
@@ -9313,7 +9316,7 @@
         <v>40</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>40</v>
@@ -9327,7 +9330,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9436,7 +9439,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9547,7 +9550,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9587,7 +9590,7 @@
       </c>
       <c r="P74" s="2"/>
       <c r="Q74" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="R74" t="s" s="2">
         <v>40</v>
@@ -9658,7 +9661,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9681,7 +9684,7 @@
         <v>40</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>226</v>
@@ -9767,7 +9770,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9878,7 +9881,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9989,7 +9992,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10100,11 +10103,11 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" t="s" s="2">
@@ -10126,13 +10129,13 @@
         <v>158</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
@@ -10161,10 +10164,10 @@
         <v>161</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="Z79" t="s" s="2">
         <v>40</v>
@@ -10182,7 +10185,7 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -10197,21 +10200,21 @@
         <v>40</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10234,13 +10237,13 @@
         <v>43</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -10291,7 +10294,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10309,18 +10312,18 @@
         <v>40</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10343,13 +10346,13 @@
         <v>40</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -10400,7 +10403,7 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -10412,7 +10415,7 @@
         <v>40</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AJ81" t="s" s="2">
         <v>253</v>
@@ -10429,7 +10432,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10538,7 +10541,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10645,10 +10648,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C84" t="s" s="2">
         <v>40</v>
@@ -10670,13 +10673,13 @@
         <v>40</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -10742,7 +10745,7 @@
         <v>107</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AK84" t="s" s="2">
         <v>40</v>
@@ -10756,10 +10759,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C85" t="s" s="2">
         <v>40</v>
@@ -10781,13 +10784,13 @@
         <v>40</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -10853,7 +10856,7 @@
         <v>107</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>40</v>
@@ -10867,11 +10870,11 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" t="s" s="2">
@@ -10896,7 +10899,7 @@
         <v>111</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M86" t="s" s="2">
         <v>113</v>
@@ -10949,7 +10952,7 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -10978,7 +10981,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11001,13 +11004,13 @@
         <v>40</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -11058,7 +11061,7 @@
         <v>40</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>51</v>
@@ -11087,7 +11090,7 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11196,7 +11199,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11307,7 +11310,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11333,10 +11336,10 @@
         <v>202</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M90" t="s" s="2">
         <v>234</v>
@@ -11404,7 +11407,7 @@
         <v>40</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AK90" t="s" s="2">
         <v>40</v>
@@ -11418,7 +11421,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11444,10 +11447,10 @@
         <v>116</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M91" t="s" s="2">
         <v>240</v>
@@ -11515,7 +11518,7 @@
         <v>40</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AK91" t="s" s="2">
         <v>40</v>
@@ -11529,7 +11532,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -11555,10 +11558,10 @@
         <v>202</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M92" t="s" s="2">
         <v>246</v>
@@ -11626,7 +11629,7 @@
         <v>40</v>
       </c>
       <c r="AJ92" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AK92" t="s" s="2">
         <v>40</v>
@@ -11640,7 +11643,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -11663,13 +11666,13 @@
         <v>40</v>
       </c>
       <c r="J93" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -11720,7 +11723,7 @@
         <v>40</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>41</v>
@@ -11738,7 +11741,7 @@
         <v>40</v>
       </c>
       <c r="AK93" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AL93" t="s" s="2">
         <v>40</v>

</xml_diff>